<commit_message>
modiied l_assignment to calculate uncertainties on sfs finished (d,p) l assignment
</commit_message>
<xml_diff>
--- a/spectroscopic_factors/excel/116Cd_d,p_117Cd_bite_2_spec_factors.xlsx
+++ b/spectroscopic_factors/excel/116Cd_d,p_117Cd_bite_2_spec_factors.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>ENERGY</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>SPECTROSCOPIC_FACTOR</t>
+  </si>
+  <si>
+    <t>ERROR</t>
   </si>
 </sst>
 </file>
@@ -380,13 +383,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -396,8 +399,11 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -405,13 +411,16 @@
         <v>1222</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>0.02070388154698714</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.05936598391918613</v>
+      </c>
+      <c r="E2">
+        <v>0.003035493077078442</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -424,8 +433,11 @@
       <c r="D3">
         <v>0.001488629564549792</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>0.0005326809152579089</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -433,13 +445,16 @@
         <v>1257</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>0.01592606256676202</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>0.04806465453323013</v>
+      </c>
+      <c r="E4">
+        <v>0.002708960911056775</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -452,8 +467,11 @@
       <c r="D5">
         <v>0.04036433381412403</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>0.001911775804863956</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -461,13 +479,16 @@
         <v>1317.043937608814</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>0.01170435764633139</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>0.01339031299261635</v>
+      </c>
+      <c r="E6">
+        <v>0.001508172562733018</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -480,8 +501,11 @@
       <c r="D7">
         <v>0.01178569060100847</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>0.001176774733969529</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -494,8 +518,11 @@
       <c r="D8">
         <v>0.03782973362001066</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>0.00186518307382544</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -508,8 +535,11 @@
       <c r="D9">
         <v>0.007023749912468884</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>0.002112894099568819</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -522,8 +552,11 @@
       <c r="D10">
         <v>0.009585676154232116</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <v>0.002449264765007386</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -536,8 +569,11 @@
       <c r="D11">
         <v>0.01127809196645715</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>0.00261466787634065</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -550,8 +586,11 @@
       <c r="D12">
         <v>0.0515690018978243</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>0.003501666092421833</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -564,8 +603,11 @@
       <c r="D13">
         <v>0.05321212116585639</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <v>0.00439895220724949</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -578,8 +620,11 @@
       <c r="D14">
         <v>0.002862574415674339</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <v>0.0006447551638369098</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -592,8 +637,11 @@
       <c r="D15">
         <v>0.01061489961681472</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <v>0.001541576703823349</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -601,13 +649,16 @@
         <v>1682.510718698463</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>0.008239776827799961</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>0.01572741592980416</v>
+      </c>
+      <c r="E16">
+        <v>0.001522266335368331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -620,8 +671,11 @@
       <c r="D17">
         <v>0.009258652181806135</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>0.004903073700746497</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -634,8 +688,11 @@
       <c r="D18">
         <v>0.003395164279459142</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <v>0.0007796941141099332</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -643,13 +700,16 @@
         <v>1763.505446394653</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>0.01117542402475309</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>0.008673820530755825</v>
+      </c>
+      <c r="E19">
+        <v>0.001461840480067992</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -657,13 +717,16 @@
         <v>1791.748218580141</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>0.01694714232486408</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>0.01461474403233252</v>
+      </c>
+      <c r="E20">
+        <v>0.001123036702029975</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -671,13 +734,16 @@
         <v>1813.127687077064</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0.006706364730149976</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>0.005752292219242671</v>
+      </c>
+      <c r="E21">
+        <v>0.0008842692873798057</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -690,8 +756,11 @@
       <c r="D22">
         <v>0.08300869419127654</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22">
+        <v>0.002141996245434148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -699,13 +768,16 @@
         <v>1880.787836939684</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>0.08111737173542628</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>0.06435848202244433</v>
+      </c>
+      <c r="E23">
+        <v>0.001741532107087278</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -718,8 +790,11 @@
       <c r="D24">
         <v>0.2134522650483264</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24">
+        <v>0.003099782478848739</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -732,8 +807,11 @@
       <c r="D25">
         <v>0.04059920257333815</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25">
+        <v>0.001743835996372207</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -741,13 +819,16 @@
         <v>2023.772546813318</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>0.06657352962528523</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>0.03374938964761337</v>
+      </c>
+      <c r="E26">
+        <v>0.001654950577338617</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -760,8 +841,11 @@
       <c r="D27">
         <v>0.01966188957209503</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27">
+        <v>0.001304340853869849</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -774,8 +858,11 @@
       <c r="D28">
         <v>0.06615520120800006</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28">
+        <v>0.002070416134208245</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -788,8 +875,11 @@
       <c r="D29">
         <v>0.0893192847289216</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29">
+        <v>0.003851816244631217</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -797,13 +887,16 @@
         <v>2139.92127208803</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D30">
-        <v>0.09198676347391112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>0.07163892755319588</v>
+      </c>
+      <c r="E30">
+        <v>0.00383757027733713</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -816,8 +909,11 @@
       <c r="D31">
         <v>0.01982164255915413</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31">
+        <v>0.001886740493001429</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -830,8 +926,11 @@
       <c r="D32">
         <v>0.2319110614053257</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32">
+        <v>0.004455258641850102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -844,8 +943,11 @@
       <c r="D33">
         <v>0.02514654160364252</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33">
+        <v>0.008940562847279374</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -853,13 +955,16 @@
         <v>2206.983121478583</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D34">
-        <v>0.04320275913614207</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>0.02677773877005402</v>
+      </c>
+      <c r="E34">
+        <v>0.006987578924655492</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -872,8 +977,11 @@
       <c r="D35">
         <v>0.1720638246895806</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35">
+        <v>0.003410544974445649</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -886,8 +994,11 @@
       <c r="D36">
         <v>0.01492680763126938</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36">
+        <v>0.002339332834741048</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -900,8 +1011,11 @@
       <c r="D37">
         <v>0.01315273679670204</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37">
+        <v>0.001012704540073741</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -914,8 +1028,11 @@
       <c r="D38">
         <v>0.01540334876412954</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38">
+        <v>0.001801517900222171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -928,8 +1045,11 @@
       <c r="D39">
         <v>0.009503742673139106</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39">
+        <v>0.001475055964619051</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -942,8 +1062,11 @@
       <c r="D40">
         <v>0.009872558380442114</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40">
+        <v>0.001466410306524519</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -956,8 +1079,11 @@
       <c r="D41">
         <v>0.003753287349912698</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41">
+        <v>0.002542866581186163</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -965,13 +1091,16 @@
         <v>2410.242626499789</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D42">
-        <v>0.005280580959234691</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>0.006157213440128234</v>
+      </c>
+      <c r="E42">
+        <v>0.002397460528171445</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -984,8 +1113,11 @@
       <c r="D43">
         <v>0.01424577719270922</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43">
+        <v>0.001018322376843115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -993,13 +1125,16 @@
         <v>2432.242029438034</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D44">
-        <v>0.003359610428048686</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>0.005819961319551851</v>
+      </c>
+      <c r="E44">
+        <v>0.0009469795172086425</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1007,13 +1142,16 @@
         <v>2454.916845899374</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D45">
-        <v>0.0229918079557914</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>0.0269225597187095</v>
+      </c>
+      <c r="E45">
+        <v>0.001863736576094903</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1021,13 +1159,16 @@
         <v>2461.621164024265</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46">
-        <v>0.01299845471365054</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>0.01410576666286996</v>
+      </c>
+      <c r="E46">
+        <v>0.001100481841451729</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1040,8 +1181,11 @@
       <c r="D47">
         <v>0.01810950692550556</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="E47">
+        <v>0.001227981137154653</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1049,80 +1193,115 @@
         <v>2491.878218119664</v>
       </c>
       <c r="C48">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>0.009110894868664498</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>0.005750758309528895</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49">
-        <v>2511.967542799203</v>
+        <v>2491.878218119664</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D49">
-        <v>0.008522098053666534</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>5.516487026791419e-15</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50">
-        <v>2521.402026059814</v>
+        <v>2511.967542799203</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D50">
-        <v>0.04104813711274746</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>0.0100360798260475</v>
+      </c>
+      <c r="E50">
+        <v>0.001343369766402542</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51">
-        <v>2532.743580491942</v>
+        <v>2521.402026059814</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D51">
-        <v>0.009188372424004214</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>0.04867836555897274</v>
+      </c>
+      <c r="E51">
+        <v>0.002802644367327954</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52">
-        <v>2542.951706183542</v>
+        <v>2532.743580491942</v>
       </c>
       <c r="C52">
         <v>3</v>
       </c>
       <c r="D52">
-        <v>0.02919350932781831</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>0.01096972208564659</v>
+      </c>
+      <c r="E52">
+        <v>0.001281034991850073</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53">
+        <v>2542.951706183542</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53">
+        <v>0.02919350932781831</v>
+      </c>
+      <c r="E53">
+        <v>0.001775660183078727</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54">
         <v>2552.6607271736</v>
       </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53">
-        <v>0.01731207601461708</v>
+      <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="D54">
+        <v>0.02048890572107748</v>
+      </c>
+      <c r="E54">
+        <v>0.001545096733683355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>